<commit_message>
08.11.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/November/All Details/07.11.2020/MC Bank Statement Sep-2020.xlsx
+++ b/2020/November/All Details/07.11.2020/MC Bank Statement Sep-2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Nov 2020" sheetId="7" r:id="rId1"/>
@@ -4649,7 +4649,7 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -10367,8 +10367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI246"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D118" sqref="D117:D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -21371,8 +21371,9 @@
     <mergeCell ref="F43:J43"/>
     <mergeCell ref="A59:B59"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="80" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>